<commit_message>
add data for practicals
</commit_message>
<xml_diff>
--- a/data/variables_names.xlsx
+++ b/data/variables_names.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>comm</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Type of region of residence  (1 = urban, 0 = rural)</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,44 +385,59 @@
     <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -696,14 +714,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80582ACE-1DBA-4D74-9234-9E1A6A89718C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="92e0090b-9daa-4f54-9b11-8d02d72818f6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="c5bdff16-9943-4a18-b570-b7b9733c27f1"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>